<commit_message>
CS_06_04_CO, CS_06_02_CO y CS_04_02_CO editados.
De todo un poco... Mi trabajo de una semana...
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion09/SolicitudGrafica_CS_04_09_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion09/SolicitudGrafica_CS_04_09_CO.xlsx
@@ -508,9 +508,6 @@
     <t>Solicitud gráfica de recurso:</t>
   </si>
   <si>
-    <t>Vertical</t>
-  </si>
-  <si>
     <t>División político-administrativa del territorio colombiano</t>
   </si>
   <si>
@@ -653,6 +650,9 @@
   </si>
   <si>
     <t>CS_04_09_CO_IMG01_small</t>
+  </si>
+  <si>
+    <t>Horizontal</t>
   </si>
 </sst>
 </file>
@@ -1584,6 +1584,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1680,8 +1682,6 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2431,9 +2431,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2471,14 +2471,14 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="92"/>
-      <c r="F2" s="84" t="s">
+      <c r="D2" s="94"/>
+      <c r="F2" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="85"/>
+      <c r="G2" s="87"/>
       <c r="H2" s="51"/>
       <c r="I2" s="51"/>
       <c r="J2" s="16"/>
@@ -2488,14 +2488,14 @@
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="93">
+      <c r="C3" s="95">
         <v>4</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="F3" s="86">
+      <c r="D3" s="96"/>
+      <c r="F3" s="88">
         <v>42076</v>
       </c>
-      <c r="G3" s="87"/>
+      <c r="G3" s="89"/>
       <c r="H3" s="51"/>
       <c r="I3" s="51"/>
       <c r="J3" s="16"/>
@@ -2505,16 +2505,16 @@
       <c r="B4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="93" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" s="94"/>
+      <c r="C4" s="95" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="96"/>
       <c r="E4" s="5"/>
       <c r="F4" s="50" t="s">
         <v>56</v>
       </c>
       <c r="G4" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H4" s="51"/>
       <c r="I4" s="51"/>
@@ -2526,10 +2526,10 @@
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="95" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" s="96"/>
+      <c r="C5" s="97" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="98"/>
       <c r="E5" s="5"/>
       <c r="F5" s="48" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2562,7 +2562,7 @@
         <v>41</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>40</v>
@@ -2580,12 +2580,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="90"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="92"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2635,20 +2635,20 @@
         <v>IMG01</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" s="27" t="str">
         <f>IF(OR(B10&lt;&gt;Ayuda!A5,J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G10" s="14" t="str">
         <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -2663,7 +2663,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="19"/>
     </row>
@@ -2673,17 +2673,17 @@
         <v>IMG02</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" s="27" t="str">
         <f t="shared" ref="C11:C22" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F11" s="14" t="str">
         <f t="shared" ref="F11:F74" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
@@ -2702,7 +2702,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K11" s="15"/>
     </row>
@@ -2712,17 +2712,17 @@
         <v>IMG03</v>
       </c>
       <c r="B12" s="77" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C12" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2741,7 +2741,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J12" s="76" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K12" s="19"/>
     </row>
@@ -2751,17 +2751,17 @@
         <v>IMG04</v>
       </c>
       <c r="B13" s="75" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C13" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F13" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2779,8 +2779,8 @@
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J13" s="115" t="s">
-        <v>156</v>
+      <c r="J13" s="84" t="s">
+        <v>155</v>
       </c>
       <c r="K13" s="19"/>
     </row>
@@ -2790,17 +2790,17 @@
         <v>IMG05</v>
       </c>
       <c r="B14" s="75" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C14" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F14" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2819,7 +2819,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K14" s="19"/>
     </row>
@@ -2829,17 +2829,17 @@
         <v>IMG06</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F15" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2858,7 +2858,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="78" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K15" s="21"/>
     </row>
@@ -2868,17 +2868,17 @@
         <v>IMG07</v>
       </c>
       <c r="B16" s="75" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C16" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F16" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2897,7 +2897,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="79" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K16" s="32"/>
     </row>
@@ -2907,17 +2907,17 @@
         <v>IMG08</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F17" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2936,7 +2936,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K17" s="21"/>
     </row>
@@ -2946,17 +2946,17 @@
         <v>IMG09</v>
       </c>
       <c r="B18" s="75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C18" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F18" s="14" t="str">
         <f t="shared" si="1"/>
@@ -2974,27 +2974,27 @@
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J18" s="116" t="s">
-        <v>171</v>
+      <c r="J18" s="85" t="s">
+        <v>170</v>
       </c>
       <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B19" s="80" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C19" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F19" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3013,26 +3013,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J19" s="79" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B20" s="75" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C20" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F20" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3051,26 +3051,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J20" s="76" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="81" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="75" t="s">
         <v>176</v>
-      </c>
-      <c r="B21" s="75" t="s">
-        <v>177</v>
       </c>
       <c r="C21" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F21" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3089,26 +3089,26 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J21" s="78" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="81" t="s">
+        <v>178</v>
+      </c>
+      <c r="B22" s="82" t="s">
         <v>179</v>
-      </c>
-      <c r="B22" s="82" t="s">
-        <v>180</v>
       </c>
       <c r="C22" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F22" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3127,25 +3127,25 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J22" s="83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K22" s="20"/>
     </row>
     <row r="23" spans="1:11" s="12" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="81" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F23" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3164,25 +3164,25 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J23" s="76" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K23" s="19"/>
     </row>
     <row r="24" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="81" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24" s="74" t="s">
         <v>185</v>
       </c>
-      <c r="B24" s="74" t="s">
-        <v>186</v>
-      </c>
       <c r="C24" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F24" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3201,25 +3201,25 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J24" s="83" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K24" s="15"/>
     </row>
     <row r="25" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="81" t="s">
+        <v>187</v>
+      </c>
+      <c r="B25" s="75" t="s">
         <v>188</v>
       </c>
-      <c r="B25" s="75" t="s">
-        <v>189</v>
-      </c>
       <c r="C25" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F25" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3238,25 +3238,25 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J25" s="83" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" s="12" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="81" t="s">
+        <v>190</v>
+      </c>
+      <c r="B26" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="B26" s="75" t="s">
-        <v>192</v>
-      </c>
       <c r="C26" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="F26" s="14" t="str">
         <f t="shared" si="1"/>
@@ -3275,7 +3275,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J26" s="83" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K26" s="19"/>
     </row>
@@ -5438,25 +5438,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="103"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="42"/>
-      <c r="C2" s="102" t="s">
+      <c r="C2" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="103"/>
-      <c r="E2" s="104"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="106"/>
       <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -5464,11 +5464,11 @@
         <v>44</v>
       </c>
       <c r="B3" s="42"/>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="109"/>
-      <c r="E3" s="110"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="112"/>
       <c r="F3" s="43"/>
       <c r="H3" s="33" t="s">
         <v>19</v>
@@ -5519,11 +5519,11 @@
       <c r="C5" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="111" t="str">
+      <c r="D5" s="113" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="112"/>
+      <c r="E5" s="114"/>
       <c r="F5" s="43"/>
       <c r="H5" s="33" t="s">
         <v>23</v>
@@ -5568,12 +5568,12 @@
       <c r="C7" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="97" t="str">
+      <c r="D7" s="99" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="97"/>
-      <c r="F7" s="98"/>
+      <c r="E7" s="99"/>
+      <c r="F7" s="100"/>
       <c r="H7" s="33" t="s">
         <v>25</v>
       </c>
@@ -5667,14 +5667,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="100"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="101"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="103"/>
       <c r="I13" s="33" t="s">
         <v>34</v>
       </c>
@@ -5707,12 +5707,12 @@
         <v>47</v>
       </c>
       <c r="B15" s="42"/>
-      <c r="C15" s="102" t="s">
+      <c r="C15" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="103"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="104"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="106"/>
       <c r="J15" s="33">
         <v>12</v>
       </c>
@@ -5752,12 +5752,12 @@
       <c r="C17" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="105" t="str">
+      <c r="D17" s="107" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="106"/>
-      <c r="F17" s="107"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="109"/>
       <c r="J17" s="33">
         <v>14</v>
       </c>
@@ -5773,12 +5773,12 @@
       <c r="C18" s="73" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="97" t="str">
+      <c r="D18" s="99" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="97"/>
-      <c r="F18" s="98"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="100"/>
       <c r="J18" s="33">
         <v>15</v>
       </c>
@@ -6169,41 +6169,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="115" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="115" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="113" t="s">
+      <c r="E1" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="115" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="113" t="s">
+      <c r="G1" s="115" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="114" t="s">
+      <c r="H1" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="113"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
+      <c r="A2" s="115"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="52" t="s">
         <v>66</v>
       </c>

</xml_diff>